<commit_message>
Feature: Seletor de Data Manual e Fix na Paginação Tomados
</commit_message>
<xml_diff>
--- a/template.xlsx
+++ b/template.xlsx
@@ -1,10 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="4" lowestEdited="4" rupBuild="4505"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="24334"/>
   <workbookPr defaultThemeVersion="124226"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice Requires="x15">
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Automação ISS\"/>
+    </mc:Choice>
+  </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8DF311ED-99DF-48F8-997B-32DE37393B50}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="30" windowWidth="15600" windowHeight="9555"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Plan1" sheetId="1" r:id="rId1"/>
@@ -12,6 +18,11 @@
     <sheet name="Plan3" sheetId="3" r:id="rId3"/>
   </sheets>
   <calcPr calcId="124519"/>
+  <extLst>
+    <ext xmlns:xlwcv="http://schemas.microsoft.com/office/spreadsheetml/2024/workbookCompatibilityVersion" uri="{D14903EA-33C4-47F7-8F05-3474C54BE107}">
+      <xlwcv:version setVersion="1"/>
+    </ext>
+  </extLst>
 </workbook>
 </file>
 
@@ -30,27 +41,27 @@
     <t>Nome</t>
   </si>
   <si>
-    <t>Empresa Exemplo LTDA</t>
-  </si>
-  <si>
-    <t>00.000.000/0001-00</t>
-  </si>
-  <si>
-    <t>123.456.789-00</t>
-  </si>
-  <si>
-    <t>senha123</t>
+    <t>05.996.122/0001-01</t>
+  </si>
+  <si>
+    <t>038.050.914-86</t>
+  </si>
+  <si>
+    <t>V1pc@rgas</t>
+  </si>
+  <si>
+    <t>Vip Cargas</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <numFmts count="2">
     <numFmt numFmtId="164" formatCode="00000000000000"/>
     <numFmt numFmtId="165" formatCode="00000000000.0"/>
   </numFmts>
-  <fonts count="4">
+  <fonts count="4" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -104,28 +115,37 @@
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="2">
+  <cellXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
   </cellXfs>
   <cellStyles count="7">
-    <cellStyle name="Hyperlink 2" xfId="5"/>
+    <cellStyle name="Hyperlink 2" xfId="5" xr:uid="{00000000-0005-0000-0000-000000000000}"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
-    <cellStyle name="Normal 2 2" xfId="1"/>
-    <cellStyle name="Normal 6" xfId="4"/>
-    <cellStyle name="Normal 7" xfId="6"/>
-    <cellStyle name="Separador de milhares 2" xfId="3"/>
-    <cellStyle name="Separador de milhares 2 2 2" xfId="2"/>
+    <cellStyle name="Normal 2 2" xfId="1" xr:uid="{00000000-0005-0000-0000-000002000000}"/>
+    <cellStyle name="Normal 6" xfId="4" xr:uid="{00000000-0005-0000-0000-000003000000}"/>
+    <cellStyle name="Normal 7" xfId="6" xr:uid="{00000000-0005-0000-0000-000004000000}"/>
+    <cellStyle name="Separador de milhares 2" xfId="3" xr:uid="{00000000-0005-0000-0000-000005000000}"/>
+    <cellStyle name="Separador de milhares 2 2 2" xfId="2" xr:uid="{00000000-0005-0000-0000-000006000000}"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium9" defaultPivotStyle="PivotStyleLight16"/>
+  <extLst>
+    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
+      <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
+    </ext>
+    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{9260A510-F301-46a8-8635-F512D64BE5F5}">
+      <x15:timelineStyles defaultTimelineStyle="TimeSlicerStyleLight1"/>
+    </ext>
+  </extLst>
 </styleSheet>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
 <a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Tema do Office">
   <a:themeElements>
-    <a:clrScheme name="Escritório">
+    <a:clrScheme name="Office">
       <a:dk1>
         <a:sysClr val="windowText" lastClr="000000"/>
       </a:dk1>
@@ -163,9 +183,9 @@
         <a:srgbClr val="800080"/>
       </a:folHlink>
     </a:clrScheme>
-    <a:fontScheme name="Escritório">
+    <a:fontScheme name="Office">
       <a:majorFont>
-        <a:latin typeface="Cambria"/>
+        <a:latin typeface="Cambria" panose="020F0302020204030204"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -197,9 +217,27 @@
         <a:font script="Mong" typeface="Mongolian Baiti"/>
         <a:font script="Viet" typeface="Times New Roman"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
+        <a:font script="Geor" typeface="Sylfaen"/>
+        <a:font script="Armn" typeface="Arial"/>
+        <a:font script="Bugi" typeface="Leelawadee UI"/>
+        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
+        <a:font script="Java" typeface="Javanese Text"/>
+        <a:font script="Lisu" typeface="Segoe UI"/>
+        <a:font script="Mymr" typeface="Myanmar Text"/>
+        <a:font script="Nkoo" typeface="Ebrima"/>
+        <a:font script="Olck" typeface="Nirmala UI"/>
+        <a:font script="Osma" typeface="Ebrima"/>
+        <a:font script="Phag" typeface="Phagspa"/>
+        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
+        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
+        <a:font script="Syre" typeface="Estrangelo Edessa"/>
+        <a:font script="Sora" typeface="Nirmala UI"/>
+        <a:font script="Tale" typeface="Microsoft Tai Le"/>
+        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
+        <a:font script="Tfng" typeface="Ebrima"/>
       </a:majorFont>
       <a:minorFont>
-        <a:latin typeface="Calibri"/>
+        <a:latin typeface="Calibri" panose="020F0502020204030204"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -231,9 +269,27 @@
         <a:font script="Mong" typeface="Mongolian Baiti"/>
         <a:font script="Viet" typeface="Arial"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
+        <a:font script="Geor" typeface="Sylfaen"/>
+        <a:font script="Armn" typeface="Arial"/>
+        <a:font script="Bugi" typeface="Leelawadee UI"/>
+        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
+        <a:font script="Java" typeface="Javanese Text"/>
+        <a:font script="Lisu" typeface="Segoe UI"/>
+        <a:font script="Mymr" typeface="Myanmar Text"/>
+        <a:font script="Nkoo" typeface="Ebrima"/>
+        <a:font script="Olck" typeface="Nirmala UI"/>
+        <a:font script="Osma" typeface="Ebrima"/>
+        <a:font script="Phag" typeface="Phagspa"/>
+        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
+        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
+        <a:font script="Syre" typeface="Estrangelo Edessa"/>
+        <a:font script="Sora" typeface="Nirmala UI"/>
+        <a:font script="Tale" typeface="Microsoft Tai Le"/>
+        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
+        <a:font script="Tfng" typeface="Ebrima"/>
       </a:minorFont>
     </a:fontScheme>
-    <a:fmtScheme name="Escritório">
+    <a:fmtScheme name="Office">
       <a:fillStyleLst>
         <a:solidFill>
           <a:schemeClr val="phClr"/>
@@ -406,14 +462,14 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:D2"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D10" sqref="D10"/>
+      <selection activeCell="C8" sqref="C8"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="24.7109375" style="1" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="18" style="1" bestFit="1" customWidth="1"/>
@@ -421,7 +477,7 @@
     <col min="4" max="4" width="17.5703125" style="1" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4">
+    <row r="1" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>3</v>
       </c>
@@ -435,44 +491,45 @@
         <v>2</v>
       </c>
     </row>
-    <row r="2" spans="1:4">
+    <row r="2" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A2" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="B2" s="2" t="s">
         <v>4</v>
       </c>
-      <c r="B2" s="1" t="s">
+      <c r="C2" s="1" t="s">
         <v>5</v>
       </c>
-      <c r="C2" s="1" t="s">
+      <c r="D2" s="1" t="s">
         <v>6</v>
-      </c>
-      <c r="D2" s="1" t="s">
-        <v>7</v>
       </c>
     </row>
   </sheetData>
   <pageMargins left="0.511811024" right="0.511811024" top="0.78740157499999996" bottom="0.78740157499999996" header="0.31496062000000002" footer="0.31496062000000002"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A1"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData/>
   <pageMargins left="0.511811024" right="0.511811024" top="0.78740157499999996" bottom="0.78740157499999996" header="0.31496062000000002" footer="0.31496062000000002"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
   <dimension ref="A1"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData/>
   <pageMargins left="0.511811024" right="0.511811024" top="0.78740157499999996" bottom="0.78740157499999996" header="0.31496062000000002" footer="0.31496062000000002"/>
 </worksheet>

</xml_diff>